<commit_message>
Updated test data for versatility
</commit_message>
<xml_diff>
--- a/FinalProject/PrototypeTestData.xlsx
+++ b/FinalProject/PrototypeTestData.xlsx
@@ -9,17 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="0" windowWidth="21570" windowHeight="8145" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="21570" windowHeight="8145" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
-    <sheet name="Customer" sheetId="1" r:id="rId1"/>
-    <sheet name="Model" sheetId="9" r:id="rId2"/>
-    <sheet name="Distributor" sheetId="10" r:id="rId3"/>
-    <sheet name="Toy" sheetId="11" r:id="rId4"/>
-    <sheet name="Registration" sheetId="12" r:id="rId5"/>
-    <sheet name="RegistrationQuestion" sheetId="13" r:id="rId6"/>
-    <sheet name="RegistrationAnswer" sheetId="14" r:id="rId7"/>
-    <sheet name="RegistrationResponse" sheetId="15" r:id="rId8"/>
+    <sheet name="1Customer" sheetId="1" r:id="rId1"/>
+    <sheet name="1Model" sheetId="9" r:id="rId2"/>
+    <sheet name="1Distributor" sheetId="10" r:id="rId3"/>
+    <sheet name="2Toy" sheetId="11" r:id="rId4"/>
+    <sheet name="2RegistrationQuestion" sheetId="13" r:id="rId5"/>
+    <sheet name="3RegistrationAnswer" sheetId="14" r:id="rId6"/>
+    <sheet name="4Registration" sheetId="12" r:id="rId7"/>
+    <sheet name="5RegistrationResponse" sheetId="15" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
@@ -2251,10 +2251,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B21"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2427,387 +2427,44 @@
         <v>73295891</v>
       </c>
     </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>11111111</v>
+      </c>
+      <c r="B22" s="1">
+        <v>73295891</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>22222222</v>
+      </c>
+      <c r="B23" s="1">
+        <v>73295891</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>33333333</v>
+      </c>
+      <c r="B24" s="1">
+        <v>73295891</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>44444444</v>
+      </c>
+      <c r="B25" s="1">
+        <v>61566272</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="4" max="4" width="14.25" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>42675336</v>
-      </c>
-      <c r="B2" s="1">
-        <v>18348</v>
-      </c>
-      <c r="C2" s="1">
-        <v>86702</v>
-      </c>
-      <c r="D2" s="2">
-        <v>41246</v>
-      </c>
-      <c r="E2" s="1">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>42464912</v>
-      </c>
-      <c r="B3" s="1">
-        <v>41233</v>
-      </c>
-      <c r="C3" s="1">
-        <v>15947</v>
-      </c>
-      <c r="D3" s="2">
-        <v>41642</v>
-      </c>
-      <c r="E3" s="1">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>92423536</v>
-      </c>
-      <c r="B4" s="1">
-        <v>74595</v>
-      </c>
-      <c r="C4" s="1">
-        <v>32420</v>
-      </c>
-      <c r="D4" s="2">
-        <v>41669</v>
-      </c>
-      <c r="E4" s="1">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>18567525</v>
-      </c>
-      <c r="B5" s="1">
-        <v>60471</v>
-      </c>
-      <c r="C5" s="1">
-        <v>56171</v>
-      </c>
-      <c r="D5" s="2">
-        <v>41154</v>
-      </c>
-      <c r="E5" s="1">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>37832480</v>
-      </c>
-      <c r="B6" s="1">
-        <v>92890</v>
-      </c>
-      <c r="C6" s="1">
-        <v>80210</v>
-      </c>
-      <c r="D6" s="2">
-        <v>41154</v>
-      </c>
-      <c r="E6" s="1">
-        <v>671</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>24784636</v>
-      </c>
-      <c r="B7" s="1">
-        <v>89580</v>
-      </c>
-      <c r="C7" s="1">
-        <v>15481</v>
-      </c>
-      <c r="D7" s="2">
-        <v>40664</v>
-      </c>
-      <c r="E7" s="1">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>34463671</v>
-      </c>
-      <c r="B8" s="1">
-        <v>33480</v>
-      </c>
-      <c r="C8" s="1">
-        <v>51578</v>
-      </c>
-      <c r="D8" s="2">
-        <v>40217</v>
-      </c>
-      <c r="E8" s="1">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>14133677</v>
-      </c>
-      <c r="B9" s="1">
-        <v>89579</v>
-      </c>
-      <c r="C9" s="1">
-        <v>46792</v>
-      </c>
-      <c r="D9" s="2">
-        <v>40224</v>
-      </c>
-      <c r="E9" s="1">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>72544274</v>
-      </c>
-      <c r="B10" s="1">
-        <v>53313</v>
-      </c>
-      <c r="C10" s="1">
-        <v>10894</v>
-      </c>
-      <c r="D10" s="2">
-        <v>42099</v>
-      </c>
-      <c r="E10" s="1">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>46714293</v>
-      </c>
-      <c r="B11" s="1">
-        <v>63156</v>
-      </c>
-      <c r="C11" s="1">
-        <v>15481</v>
-      </c>
-      <c r="D11" s="2">
-        <v>42191</v>
-      </c>
-      <c r="E11" s="1">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>86759623</v>
-      </c>
-      <c r="B12" s="1">
-        <v>42062</v>
-      </c>
-      <c r="C12" s="1">
-        <v>56171</v>
-      </c>
-      <c r="D12" s="2">
-        <v>41206</v>
-      </c>
-      <c r="E12" s="1">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>52377834</v>
-      </c>
-      <c r="B13" s="1">
-        <v>87869</v>
-      </c>
-      <c r="C13" s="1">
-        <v>46792</v>
-      </c>
-      <c r="D13" s="2">
-        <v>42219</v>
-      </c>
-      <c r="E13" s="1">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>50488423</v>
-      </c>
-      <c r="B14" s="1">
-        <v>89491</v>
-      </c>
-      <c r="C14" s="1">
-        <v>15481</v>
-      </c>
-      <c r="D14" s="2">
-        <v>42254</v>
-      </c>
-      <c r="E14" s="1">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>82513149</v>
-      </c>
-      <c r="B15" s="1">
-        <v>46948</v>
-      </c>
-      <c r="C15" s="1">
-        <v>46792</v>
-      </c>
-      <c r="D15" s="2">
-        <v>41814</v>
-      </c>
-      <c r="E15" s="1">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>80830234</v>
-      </c>
-      <c r="B16" s="1">
-        <v>72090</v>
-      </c>
-      <c r="C16" s="1">
-        <v>15481</v>
-      </c>
-      <c r="D16" s="2">
-        <v>41815</v>
-      </c>
-      <c r="E16" s="1">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>21847715</v>
-      </c>
-      <c r="B17" s="1">
-        <v>39811</v>
-      </c>
-      <c r="C17" s="1">
-        <v>46792</v>
-      </c>
-      <c r="D17" s="2">
-        <v>41816</v>
-      </c>
-      <c r="E17" s="1">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>86928760</v>
-      </c>
-      <c r="B18" s="1">
-        <v>37534</v>
-      </c>
-      <c r="C18" s="1">
-        <v>46792</v>
-      </c>
-      <c r="D18" s="2">
-        <v>41817</v>
-      </c>
-      <c r="E18" s="1">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>11293419</v>
-      </c>
-      <c r="B19" s="1">
-        <v>27457</v>
-      </c>
-      <c r="C19" s="1">
-        <v>56171</v>
-      </c>
-      <c r="D19" s="2">
-        <v>41336</v>
-      </c>
-      <c r="E19" s="1">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>24896934</v>
-      </c>
-      <c r="B20" s="1">
-        <v>74150</v>
-      </c>
-      <c r="C20" s="1">
-        <v>46792</v>
-      </c>
-      <c r="D20" s="2">
-        <v>42371</v>
-      </c>
-      <c r="E20" s="1">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>65887539</v>
-      </c>
-      <c r="B21" s="1">
-        <v>40248</v>
-      </c>
-      <c r="C21" s="1">
-        <v>46792</v>
-      </c>
-      <c r="D21" s="2">
-        <v>41097</v>
-      </c>
-      <c r="E21" s="1">
-        <v>296</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
@@ -2926,15 +2583,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C42"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="28.625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
@@ -3396,6 +3056,449 @@
       </c>
       <c r="C42" s="1">
         <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="14.25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>42675336</v>
+      </c>
+      <c r="B2" s="1">
+        <v>18348</v>
+      </c>
+      <c r="C2" s="1">
+        <v>86702</v>
+      </c>
+      <c r="D2" s="2">
+        <v>41246</v>
+      </c>
+      <c r="E2" s="1">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>42464912</v>
+      </c>
+      <c r="B3" s="1">
+        <v>41233</v>
+      </c>
+      <c r="C3" s="1">
+        <v>15947</v>
+      </c>
+      <c r="D3" s="2">
+        <v>41642</v>
+      </c>
+      <c r="E3" s="1">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>92423536</v>
+      </c>
+      <c r="B4" s="1">
+        <v>74595</v>
+      </c>
+      <c r="C4" s="1">
+        <v>32420</v>
+      </c>
+      <c r="D4" s="2">
+        <v>41669</v>
+      </c>
+      <c r="E4" s="1">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>18567525</v>
+      </c>
+      <c r="B5" s="1">
+        <v>60471</v>
+      </c>
+      <c r="C5" s="1">
+        <v>56171</v>
+      </c>
+      <c r="D5" s="2">
+        <v>41154</v>
+      </c>
+      <c r="E5" s="1">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>37832480</v>
+      </c>
+      <c r="B6" s="1">
+        <v>92890</v>
+      </c>
+      <c r="C6" s="1">
+        <v>80210</v>
+      </c>
+      <c r="D6" s="2">
+        <v>41154</v>
+      </c>
+      <c r="E6" s="1">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>24784636</v>
+      </c>
+      <c r="B7" s="1">
+        <v>89580</v>
+      </c>
+      <c r="C7" s="1">
+        <v>15481</v>
+      </c>
+      <c r="D7" s="2">
+        <v>40664</v>
+      </c>
+      <c r="E7" s="1">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>34463671</v>
+      </c>
+      <c r="B8" s="1">
+        <v>33480</v>
+      </c>
+      <c r="C8" s="1">
+        <v>51578</v>
+      </c>
+      <c r="D8" s="2">
+        <v>40217</v>
+      </c>
+      <c r="E8" s="1">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>14133677</v>
+      </c>
+      <c r="B9" s="1">
+        <v>89579</v>
+      </c>
+      <c r="C9" s="1">
+        <v>46792</v>
+      </c>
+      <c r="D9" s="2">
+        <v>40224</v>
+      </c>
+      <c r="E9" s="1">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>72544274</v>
+      </c>
+      <c r="B10" s="1">
+        <v>53313</v>
+      </c>
+      <c r="C10" s="1">
+        <v>10894</v>
+      </c>
+      <c r="D10" s="2">
+        <v>42099</v>
+      </c>
+      <c r="E10" s="1">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>46714293</v>
+      </c>
+      <c r="B11" s="1">
+        <v>63156</v>
+      </c>
+      <c r="C11" s="1">
+        <v>15481</v>
+      </c>
+      <c r="D11" s="2">
+        <v>42191</v>
+      </c>
+      <c r="E11" s="1">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>86759623</v>
+      </c>
+      <c r="B12" s="1">
+        <v>42062</v>
+      </c>
+      <c r="C12" s="1">
+        <v>56171</v>
+      </c>
+      <c r="D12" s="2">
+        <v>41206</v>
+      </c>
+      <c r="E12" s="1">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>52377834</v>
+      </c>
+      <c r="B13" s="1">
+        <v>87869</v>
+      </c>
+      <c r="C13" s="1">
+        <v>46792</v>
+      </c>
+      <c r="D13" s="2">
+        <v>42219</v>
+      </c>
+      <c r="E13" s="1">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>50488423</v>
+      </c>
+      <c r="B14" s="1">
+        <v>89491</v>
+      </c>
+      <c r="C14" s="1">
+        <v>15481</v>
+      </c>
+      <c r="D14" s="2">
+        <v>42254</v>
+      </c>
+      <c r="E14" s="1">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>82513149</v>
+      </c>
+      <c r="B15" s="1">
+        <v>46948</v>
+      </c>
+      <c r="C15" s="1">
+        <v>46792</v>
+      </c>
+      <c r="D15" s="2">
+        <v>41814</v>
+      </c>
+      <c r="E15" s="1">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>80830234</v>
+      </c>
+      <c r="B16" s="1">
+        <v>72090</v>
+      </c>
+      <c r="C16" s="1">
+        <v>15481</v>
+      </c>
+      <c r="D16" s="2">
+        <v>41815</v>
+      </c>
+      <c r="E16" s="1">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>21847715</v>
+      </c>
+      <c r="B17" s="1">
+        <v>39811</v>
+      </c>
+      <c r="C17" s="1">
+        <v>46792</v>
+      </c>
+      <c r="D17" s="2">
+        <v>41816</v>
+      </c>
+      <c r="E17" s="1">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>86928760</v>
+      </c>
+      <c r="B18" s="1">
+        <v>37534</v>
+      </c>
+      <c r="C18" s="1">
+        <v>46792</v>
+      </c>
+      <c r="D18" s="2">
+        <v>41817</v>
+      </c>
+      <c r="E18" s="1">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>11293419</v>
+      </c>
+      <c r="B19" s="1">
+        <v>27457</v>
+      </c>
+      <c r="C19" s="1">
+        <v>56171</v>
+      </c>
+      <c r="D19" s="2">
+        <v>41336</v>
+      </c>
+      <c r="E19" s="1">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>24896934</v>
+      </c>
+      <c r="B20" s="1">
+        <v>74150</v>
+      </c>
+      <c r="C20" s="1">
+        <v>46792</v>
+      </c>
+      <c r="D20" s="2">
+        <v>42371</v>
+      </c>
+      <c r="E20" s="1">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>65887539</v>
+      </c>
+      <c r="B21" s="1">
+        <v>40248</v>
+      </c>
+      <c r="C21" s="1">
+        <v>46792</v>
+      </c>
+      <c r="D21" s="2">
+        <v>41097</v>
+      </c>
+      <c r="E21" s="1">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>11111111</v>
+      </c>
+      <c r="B22" s="1">
+        <v>74150</v>
+      </c>
+      <c r="C22" s="1">
+        <v>56171</v>
+      </c>
+      <c r="D22" s="2">
+        <v>41669</v>
+      </c>
+      <c r="E22" s="3">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>22222222</v>
+      </c>
+      <c r="B23" s="1">
+        <v>27457</v>
+      </c>
+      <c r="C23" s="1">
+        <v>10894</v>
+      </c>
+      <c r="D23" s="2">
+        <v>41097</v>
+      </c>
+      <c r="E23" s="3">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>33333333</v>
+      </c>
+      <c r="B24" s="1">
+        <v>37534</v>
+      </c>
+      <c r="C24" s="1">
+        <v>46792</v>
+      </c>
+      <c r="D24" s="2">
+        <v>42219</v>
+      </c>
+      <c r="E24" s="3">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>44444444</v>
+      </c>
+      <c r="B25" s="1">
+        <v>74150</v>
+      </c>
+      <c r="C25" s="1">
+        <v>10894</v>
+      </c>
+      <c r="D25" s="2">
+        <v>41814</v>
+      </c>
+      <c r="E25" s="3">
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -3405,10 +3508,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C241"/>
+  <dimension ref="A1:C278"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C241"/>
+    <sheetView tabSelected="1" topLeftCell="A256" workbookViewId="0">
+      <selection activeCell="B277" sqref="B277"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3426,12 +3529,12 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <f t="shared" ref="A2:A241" si="0">ROW()</f>
+        <f t="shared" ref="A2:A242" si="0">ROW()</f>
         <v>2</v>
       </c>
       <c r="B2" s="4">
         <f ca="1">RANDBETWEEN(1,6)</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1">
         <v>42675336</v>
@@ -3444,7 +3547,7 @@
       </c>
       <c r="B3" s="4">
         <f ca="1">RANDBETWEEN(11,12)</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1">
         <v>42675336</v>
@@ -3470,7 +3573,7 @@
       </c>
       <c r="B5" s="4">
         <f ca="1">RANDBETWEEN(31,34)</f>
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C5" s="1">
         <v>42675336</v>
@@ -3483,7 +3586,7 @@
       </c>
       <c r="B6" s="4">
         <f ca="1">RANDBETWEEN(41,44)</f>
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C6" s="1">
         <v>42675336</v>
@@ -3496,7 +3599,7 @@
       </c>
       <c r="B7" s="4">
         <f ca="1">RANDBETWEEN(50,59)</f>
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C7" s="1">
         <v>42675336</v>
@@ -3509,7 +3612,7 @@
       </c>
       <c r="B8" s="4">
         <f ca="1">RANDBETWEEN(61,63)</f>
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C8" s="1">
         <v>42675336</v>
@@ -3522,7 +3625,7 @@
       </c>
       <c r="B9" s="4">
         <f ca="1">RANDBETWEEN(71,72)</f>
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C9" s="1">
         <v>42675336</v>
@@ -3535,7 +3638,7 @@
       </c>
       <c r="B10" s="4">
         <f ca="1">RANDBETWEEN(81,82)</f>
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C10" s="1">
         <v>42675336</v>
@@ -3548,7 +3651,7 @@
       </c>
       <c r="B11" s="4">
         <f ca="1">RANDBETWEEN(91,92)</f>
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C11" s="1">
         <v>42675336</v>
@@ -3574,7 +3677,7 @@
       </c>
       <c r="B13" s="4">
         <f ca="1">RANDBETWEEN(111,112)</f>
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C13" s="1">
         <v>42675336</v>
@@ -3587,7 +3690,7 @@
       </c>
       <c r="B14" s="4">
         <f ca="1">RANDBETWEEN(1,6)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C14" s="1">
         <v>42464912</v>
@@ -3613,7 +3716,7 @@
       </c>
       <c r="B16" s="4">
         <f ca="1">RANDBETWEEN(21,22)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C16" s="1">
         <v>42464912</v>
@@ -3626,7 +3729,7 @@
       </c>
       <c r="B17" s="4">
         <f ca="1">RANDBETWEEN(31,34)</f>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C17" s="1">
         <v>42464912</v>
@@ -3639,7 +3742,7 @@
       </c>
       <c r="B18" s="4">
         <f ca="1">RANDBETWEEN(41,44)</f>
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C18" s="1">
         <v>42464912</v>
@@ -3652,7 +3755,7 @@
       </c>
       <c r="B19" s="4">
         <f ca="1">RANDBETWEEN(50,59)</f>
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C19" s="1">
         <v>42464912</v>
@@ -3665,7 +3768,7 @@
       </c>
       <c r="B20" s="4">
         <f ca="1">RANDBETWEEN(61,63)</f>
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C20" s="1">
         <v>42464912</v>
@@ -3678,7 +3781,7 @@
       </c>
       <c r="B21" s="4">
         <f ca="1">RANDBETWEEN(71,72)</f>
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C21" s="1">
         <v>42464912</v>
@@ -3691,7 +3794,7 @@
       </c>
       <c r="B22" s="4">
         <f ca="1">RANDBETWEEN(81,82)</f>
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C22" s="1">
         <v>42464912</v>
@@ -3717,7 +3820,7 @@
       </c>
       <c r="B24" s="4">
         <f ca="1">RANDBETWEEN(101,102)</f>
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C24" s="1">
         <v>42464912</v>
@@ -3730,7 +3833,7 @@
       </c>
       <c r="B25" s="4">
         <f ca="1">RANDBETWEEN(111,112)</f>
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C25" s="1">
         <v>42464912</v>
@@ -3743,7 +3846,7 @@
       </c>
       <c r="B26" s="5">
         <f ca="1">RANDBETWEEN(1,6)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C26" s="1">
         <v>92423536</v>
@@ -3769,7 +3872,7 @@
       </c>
       <c r="B28" s="5">
         <f ca="1">RANDBETWEEN(21,22)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C28" s="1">
         <v>92423536</v>
@@ -3795,7 +3898,7 @@
       </c>
       <c r="B30" s="5">
         <f ca="1">RANDBETWEEN(41,44)</f>
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C30" s="1">
         <v>92423536</v>
@@ -3808,7 +3911,7 @@
       </c>
       <c r="B31" s="5">
         <f ca="1">RANDBETWEEN(50,59)</f>
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C31" s="1">
         <v>92423536</v>
@@ -3821,7 +3924,7 @@
       </c>
       <c r="B32" s="5">
         <f ca="1">RANDBETWEEN(61,63)</f>
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C32" s="1">
         <v>92423536</v>
@@ -3834,7 +3937,7 @@
       </c>
       <c r="B33" s="5">
         <f ca="1">RANDBETWEEN(71,72)</f>
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C33" s="1">
         <v>92423536</v>
@@ -3873,7 +3976,7 @@
       </c>
       <c r="B36" s="5">
         <f ca="1">RANDBETWEEN(101,102)</f>
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C36" s="1">
         <v>92423536</v>
@@ -3899,7 +4002,7 @@
       </c>
       <c r="B38" s="5">
         <f ca="1">RANDBETWEEN(1,6)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C38" s="1">
         <v>18567525</v>
@@ -3912,7 +4015,7 @@
       </c>
       <c r="B39" s="5">
         <f ca="1">RANDBETWEEN(11,12)</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C39" s="1">
         <v>18567525</v>
@@ -3925,7 +4028,7 @@
       </c>
       <c r="B40" s="5">
         <f ca="1">RANDBETWEEN(21,22)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C40" s="1">
         <v>18567525</v>
@@ -3938,7 +4041,7 @@
       </c>
       <c r="B41" s="5">
         <f ca="1">RANDBETWEEN(31,34)</f>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C41" s="1">
         <v>18567525</v>
@@ -3951,7 +4054,7 @@
       </c>
       <c r="B42" s="5">
         <f ca="1">RANDBETWEEN(41,44)</f>
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C42" s="1">
         <v>18567525</v>
@@ -4029,7 +4132,7 @@
       </c>
       <c r="B48" s="5">
         <f ca="1">RANDBETWEEN(101,102)</f>
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C48" s="1">
         <v>18567525</v>
@@ -4055,7 +4158,7 @@
       </c>
       <c r="B50" s="5">
         <f ca="1">RANDBETWEEN(1,6)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C50" s="1">
         <v>37832480</v>
@@ -4068,7 +4171,7 @@
       </c>
       <c r="B51" s="5">
         <f ca="1">RANDBETWEEN(11,12)</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C51" s="1">
         <v>37832480</v>
@@ -4094,7 +4197,7 @@
       </c>
       <c r="B53" s="5">
         <f ca="1">RANDBETWEEN(31,34)</f>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C53" s="1">
         <v>37832480</v>
@@ -4172,7 +4275,7 @@
       </c>
       <c r="B59" s="5">
         <f ca="1">RANDBETWEEN(91,92)</f>
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C59" s="1">
         <v>37832480</v>
@@ -4185,7 +4288,7 @@
       </c>
       <c r="B60" s="5">
         <f ca="1">RANDBETWEEN(101,102)</f>
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C60" s="1">
         <v>37832480</v>
@@ -4198,7 +4301,7 @@
       </c>
       <c r="B61" s="5">
         <f ca="1">RANDBETWEEN(111,112)</f>
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C61" s="1">
         <v>37832480</v>
@@ -4211,7 +4314,7 @@
       </c>
       <c r="B62" s="5">
         <f ca="1">RANDBETWEEN(1,6)</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C62" s="1">
         <v>24784636</v>
@@ -4237,7 +4340,7 @@
       </c>
       <c r="B64" s="5">
         <f ca="1">RANDBETWEEN(21,22)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C64" s="1">
         <v>24784636</v>
@@ -4250,7 +4353,7 @@
       </c>
       <c r="B65" s="5">
         <f ca="1">RANDBETWEEN(31,34)</f>
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C65" s="1">
         <v>24784636</v>
@@ -4263,7 +4366,7 @@
       </c>
       <c r="B66" s="5">
         <f ca="1">RANDBETWEEN(41,44)</f>
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C66" s="1">
         <v>24784636</v>
@@ -4276,7 +4379,7 @@
       </c>
       <c r="B67" s="5">
         <f ca="1">RANDBETWEEN(50,59)</f>
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C67" s="1">
         <v>24784636</v>
@@ -4289,7 +4392,7 @@
       </c>
       <c r="B68" s="5">
         <f ca="1">RANDBETWEEN(61,63)</f>
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C68" s="1">
         <v>24784636</v>
@@ -4302,7 +4405,7 @@
       </c>
       <c r="B69" s="5">
         <f ca="1">RANDBETWEEN(71,72)</f>
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C69" s="1">
         <v>24784636</v>
@@ -4315,7 +4418,7 @@
       </c>
       <c r="B70" s="5">
         <f ca="1">RANDBETWEEN(81,82)</f>
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C70" s="1">
         <v>24784636</v>
@@ -4341,7 +4444,7 @@
       </c>
       <c r="B72" s="5">
         <f ca="1">RANDBETWEEN(101,102)</f>
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C72" s="1">
         <v>24784636</v>
@@ -4354,7 +4457,7 @@
       </c>
       <c r="B73" s="5">
         <f ca="1">RANDBETWEEN(111,112)</f>
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C73" s="1">
         <v>24784636</v>
@@ -4393,7 +4496,7 @@
       </c>
       <c r="B76" s="5">
         <f ca="1">RANDBETWEEN(21,22)</f>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C76" s="1">
         <v>34463671</v>
@@ -4406,7 +4509,7 @@
       </c>
       <c r="B77" s="5">
         <f ca="1">RANDBETWEEN(31,34)</f>
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C77" s="1">
         <v>34463671</v>
@@ -4419,7 +4522,7 @@
       </c>
       <c r="B78" s="5">
         <f ca="1">RANDBETWEEN(41,44)</f>
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C78" s="1">
         <v>34463671</v>
@@ -4432,7 +4535,7 @@
       </c>
       <c r="B79" s="5">
         <f ca="1">RANDBETWEEN(50,59)</f>
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C79" s="1">
         <v>34463671</v>
@@ -4497,7 +4600,7 @@
       </c>
       <c r="B84" s="5">
         <f ca="1">RANDBETWEEN(101,102)</f>
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C84" s="1">
         <v>34463671</v>
@@ -4510,7 +4613,7 @@
       </c>
       <c r="B85" s="5">
         <f ca="1">RANDBETWEEN(111,112)</f>
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C85" s="1">
         <v>34463671</v>
@@ -4523,7 +4626,7 @@
       </c>
       <c r="B86" s="5">
         <f ca="1">RANDBETWEEN(1,6)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C86" s="1">
         <v>14133677</v>
@@ -4536,7 +4639,7 @@
       </c>
       <c r="B87" s="5">
         <f ca="1">RANDBETWEEN(11,12)</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C87" s="1">
         <v>14133677</v>
@@ -4575,7 +4678,7 @@
       </c>
       <c r="B90" s="5">
         <f ca="1">RANDBETWEEN(41,44)</f>
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C90" s="1">
         <v>14133677</v>
@@ -4588,7 +4691,7 @@
       </c>
       <c r="B91" s="5">
         <f ca="1">RANDBETWEEN(50,59)</f>
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C91" s="1">
         <v>14133677</v>
@@ -4640,7 +4743,7 @@
       </c>
       <c r="B95" s="5">
         <f ca="1">RANDBETWEEN(91,92)</f>
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C95" s="1">
         <v>14133677</v>
@@ -4653,7 +4756,7 @@
       </c>
       <c r="B96" s="5">
         <f ca="1">RANDBETWEEN(101,102)</f>
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C96" s="1">
         <v>14133677</v>
@@ -4679,7 +4782,7 @@
       </c>
       <c r="B98" s="5">
         <f ca="1">RANDBETWEEN(1,6)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C98" s="1">
         <v>72544274</v>
@@ -4705,7 +4808,7 @@
       </c>
       <c r="B100" s="5">
         <f ca="1">RANDBETWEEN(21,22)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C100" s="1">
         <v>72544274</v>
@@ -4731,7 +4834,7 @@
       </c>
       <c r="B102" s="5">
         <f ca="1">RANDBETWEEN(41,44)</f>
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C102" s="1">
         <v>72544274</v>
@@ -4744,7 +4847,7 @@
       </c>
       <c r="B103" s="5">
         <f ca="1">RANDBETWEEN(50,59)</f>
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C103" s="1">
         <v>72544274</v>
@@ -4809,7 +4912,7 @@
       </c>
       <c r="B108" s="5">
         <f ca="1">RANDBETWEEN(101,102)</f>
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C108" s="1">
         <v>72544274</v>
@@ -4822,7 +4925,7 @@
       </c>
       <c r="B109" s="5">
         <f ca="1">RANDBETWEEN(111,112)</f>
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C109" s="1">
         <v>72544274</v>
@@ -4835,7 +4938,7 @@
       </c>
       <c r="B110" s="5">
         <f ca="1">RANDBETWEEN(1,6)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C110" s="1">
         <v>46714293</v>
@@ -4861,7 +4964,7 @@
       </c>
       <c r="B112" s="5">
         <f ca="1">RANDBETWEEN(21,22)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C112" s="1">
         <v>46714293</v>
@@ -4874,7 +4977,7 @@
       </c>
       <c r="B113" s="5">
         <f ca="1">RANDBETWEEN(31,34)</f>
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C113" s="1">
         <v>46714293</v>
@@ -4887,7 +4990,7 @@
       </c>
       <c r="B114" s="5">
         <f ca="1">RANDBETWEEN(41,44)</f>
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C114" s="1">
         <v>46714293</v>
@@ -4900,7 +5003,7 @@
       </c>
       <c r="B115" s="5">
         <f ca="1">RANDBETWEEN(50,59)</f>
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C115" s="1">
         <v>46714293</v>
@@ -4965,7 +5068,7 @@
       </c>
       <c r="B120" s="5">
         <f ca="1">RANDBETWEEN(101,102)</f>
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C120" s="1">
         <v>46714293</v>
@@ -4978,7 +5081,7 @@
       </c>
       <c r="B121" s="5">
         <f ca="1">RANDBETWEEN(111,112)</f>
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C121" s="1">
         <v>46714293</v>
@@ -4991,7 +5094,7 @@
       </c>
       <c r="B122" s="5">
         <f ca="1">RANDBETWEEN(1,6)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C122" s="1">
         <v>86759623</v>
@@ -5004,7 +5107,7 @@
       </c>
       <c r="B123" s="5">
         <f ca="1">RANDBETWEEN(11,12)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C123" s="1">
         <v>86759623</v>
@@ -5017,7 +5120,7 @@
       </c>
       <c r="B124" s="5">
         <f ca="1">RANDBETWEEN(21,22)</f>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C124" s="1">
         <v>86759623</v>
@@ -5030,7 +5133,7 @@
       </c>
       <c r="B125" s="5">
         <f ca="1">RANDBETWEEN(31,34)</f>
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C125" s="1">
         <v>86759623</v>
@@ -5043,7 +5146,7 @@
       </c>
       <c r="B126" s="5">
         <f ca="1">RANDBETWEEN(41,44)</f>
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C126" s="1">
         <v>86759623</v>
@@ -5056,7 +5159,7 @@
       </c>
       <c r="B127" s="5">
         <f ca="1">RANDBETWEEN(50,59)</f>
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C127" s="1">
         <v>86759623</v>
@@ -5069,7 +5172,7 @@
       </c>
       <c r="B128" s="5">
         <f ca="1">RANDBETWEEN(61,63)</f>
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C128" s="1">
         <v>86759623</v>
@@ -5095,7 +5198,7 @@
       </c>
       <c r="B130" s="5">
         <f ca="1">RANDBETWEEN(81,82)</f>
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C130" s="1">
         <v>86759623</v>
@@ -5134,7 +5237,7 @@
       </c>
       <c r="B133" s="5">
         <f ca="1">RANDBETWEEN(111,112)</f>
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C133" s="1">
         <v>86759623</v>
@@ -5147,7 +5250,7 @@
       </c>
       <c r="B134" s="5">
         <f ca="1">RANDBETWEEN(1,6)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C134" s="1">
         <v>52377834</v>
@@ -5186,7 +5289,7 @@
       </c>
       <c r="B137" s="5">
         <f ca="1">RANDBETWEEN(31,34)</f>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C137" s="1">
         <v>52377834</v>
@@ -5199,7 +5302,7 @@
       </c>
       <c r="B138" s="5">
         <f ca="1">RANDBETWEEN(41,44)</f>
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C138" s="1">
         <v>52377834</v>
@@ -5212,7 +5315,7 @@
       </c>
       <c r="B139" s="5">
         <f ca="1">RANDBETWEEN(50,59)</f>
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C139" s="1">
         <v>52377834</v>
@@ -5225,7 +5328,7 @@
       </c>
       <c r="B140" s="5">
         <f ca="1">RANDBETWEEN(61,63)</f>
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C140" s="1">
         <v>52377834</v>
@@ -5238,7 +5341,7 @@
       </c>
       <c r="B141" s="5">
         <f ca="1">RANDBETWEEN(71,72)</f>
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C141" s="1">
         <v>52377834</v>
@@ -5264,7 +5367,7 @@
       </c>
       <c r="B143" s="5">
         <f ca="1">RANDBETWEEN(91,92)</f>
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C143" s="1">
         <v>52377834</v>
@@ -5290,7 +5393,7 @@
       </c>
       <c r="B145" s="5">
         <f ca="1">RANDBETWEEN(111,112)</f>
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C145" s="1">
         <v>52377834</v>
@@ -5303,7 +5406,7 @@
       </c>
       <c r="B146" s="5">
         <f ca="1">RANDBETWEEN(1,6)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C146" s="1">
         <v>50488423</v>
@@ -5316,7 +5419,7 @@
       </c>
       <c r="B147" s="5">
         <f ca="1">RANDBETWEEN(11,12)</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C147" s="1">
         <v>50488423</v>
@@ -5329,7 +5432,7 @@
       </c>
       <c r="B148" s="5">
         <f ca="1">RANDBETWEEN(21,22)</f>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C148" s="1">
         <v>50488423</v>
@@ -5381,7 +5484,7 @@
       </c>
       <c r="B152" s="5">
         <f ca="1">RANDBETWEEN(61,63)</f>
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C152" s="1">
         <v>50488423</v>
@@ -5394,7 +5497,7 @@
       </c>
       <c r="B153" s="5">
         <f ca="1">RANDBETWEEN(71,72)</f>
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C153" s="1">
         <v>50488423</v>
@@ -5407,7 +5510,7 @@
       </c>
       <c r="B154" s="5">
         <f ca="1">RANDBETWEEN(81,82)</f>
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C154" s="1">
         <v>50488423</v>
@@ -5433,7 +5536,7 @@
       </c>
       <c r="B156" s="5">
         <f ca="1">RANDBETWEEN(101,102)</f>
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C156" s="1">
         <v>50488423</v>
@@ -5446,7 +5549,7 @@
       </c>
       <c r="B157" s="5">
         <f ca="1">RANDBETWEEN(111,112)</f>
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C157" s="1">
         <v>50488423</v>
@@ -5459,7 +5562,7 @@
       </c>
       <c r="B158" s="5">
         <f ca="1">RANDBETWEEN(1,6)</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C158" s="1">
         <v>82513149</v>
@@ -5498,7 +5601,7 @@
       </c>
       <c r="B161" s="5">
         <f ca="1">RANDBETWEEN(31,34)</f>
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C161" s="1">
         <v>82513149</v>
@@ -5524,7 +5627,7 @@
       </c>
       <c r="B163" s="5">
         <f ca="1">RANDBETWEEN(50,59)</f>
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C163" s="1">
         <v>82513149</v>
@@ -5550,7 +5653,7 @@
       </c>
       <c r="B165" s="5">
         <f ca="1">RANDBETWEEN(71,72)</f>
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C165" s="1">
         <v>82513149</v>
@@ -5576,7 +5679,7 @@
       </c>
       <c r="B167" s="5">
         <f ca="1">RANDBETWEEN(91,92)</f>
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C167" s="1">
         <v>82513149</v>
@@ -5602,7 +5705,7 @@
       </c>
       <c r="B169" s="5">
         <f ca="1">RANDBETWEEN(111,112)</f>
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C169" s="1">
         <v>82513149</v>
@@ -5615,7 +5718,7 @@
       </c>
       <c r="B170" s="5">
         <f ca="1">RANDBETWEEN(1,6)</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C170" s="1">
         <v>80830234</v>
@@ -5628,7 +5731,7 @@
       </c>
       <c r="B171" s="5">
         <f ca="1">RANDBETWEEN(11,12)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C171" s="1">
         <v>80830234</v>
@@ -5641,7 +5744,7 @@
       </c>
       <c r="B172" s="5">
         <f ca="1">RANDBETWEEN(21,22)</f>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C172" s="1">
         <v>80830234</v>
@@ -5667,7 +5770,7 @@
       </c>
       <c r="B174" s="5">
         <f ca="1">RANDBETWEEN(41,44)</f>
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C174" s="1">
         <v>80830234</v>
@@ -5680,7 +5783,7 @@
       </c>
       <c r="B175" s="5">
         <f ca="1">RANDBETWEEN(50,59)</f>
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C175" s="1">
         <v>80830234</v>
@@ -5693,7 +5796,7 @@
       </c>
       <c r="B176" s="5">
         <f ca="1">RANDBETWEEN(61,63)</f>
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C176" s="1">
         <v>80830234</v>
@@ -5732,7 +5835,7 @@
       </c>
       <c r="B179" s="5">
         <f ca="1">RANDBETWEEN(91,92)</f>
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C179" s="1">
         <v>80830234</v>
@@ -5745,7 +5848,7 @@
       </c>
       <c r="B180" s="5">
         <f ca="1">RANDBETWEEN(101,102)</f>
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C180" s="1">
         <v>80830234</v>
@@ -5771,7 +5874,7 @@
       </c>
       <c r="B182" s="5">
         <f ca="1">RANDBETWEEN(1,6)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C182" s="1">
         <v>21847715</v>
@@ -5797,7 +5900,7 @@
       </c>
       <c r="B184" s="5">
         <f ca="1">RANDBETWEEN(21,22)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C184" s="1">
         <v>21847715</v>
@@ -5810,7 +5913,7 @@
       </c>
       <c r="B185" s="5">
         <f ca="1">RANDBETWEEN(31,34)</f>
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C185" s="1">
         <v>21847715</v>
@@ -5823,7 +5926,7 @@
       </c>
       <c r="B186" s="5">
         <f ca="1">RANDBETWEEN(41,44)</f>
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C186" s="1">
         <v>21847715</v>
@@ -5836,7 +5939,7 @@
       </c>
       <c r="B187" s="5">
         <f ca="1">RANDBETWEEN(50,59)</f>
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C187" s="1">
         <v>21847715</v>
@@ -5862,7 +5965,7 @@
       </c>
       <c r="B189" s="5">
         <f ca="1">RANDBETWEEN(71,72)</f>
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C189" s="1">
         <v>21847715</v>
@@ -5875,7 +5978,7 @@
       </c>
       <c r="B190" s="5">
         <f ca="1">RANDBETWEEN(81,82)</f>
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C190" s="1">
         <v>21847715</v>
@@ -5914,7 +6017,7 @@
       </c>
       <c r="B193" s="5">
         <f ca="1">RANDBETWEEN(111,112)</f>
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C193" s="1">
         <v>21847715</v>
@@ -5927,7 +6030,7 @@
       </c>
       <c r="B194" s="5">
         <f ca="1">RANDBETWEEN(1,6)</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C194" s="1">
         <v>86928760</v>
@@ -5940,7 +6043,7 @@
       </c>
       <c r="B195" s="5">
         <f ca="1">RANDBETWEEN(11,12)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C195" s="1">
         <v>86928760</v>
@@ -5966,7 +6069,7 @@
       </c>
       <c r="B197" s="5">
         <f ca="1">RANDBETWEEN(31,34)</f>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C197" s="1">
         <v>86928760</v>
@@ -5979,7 +6082,7 @@
       </c>
       <c r="B198" s="5">
         <f ca="1">RANDBETWEEN(41,44)</f>
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C198" s="1">
         <v>86928760</v>
@@ -5992,7 +6095,7 @@
       </c>
       <c r="B199" s="5">
         <f ca="1">RANDBETWEEN(50,59)</f>
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="C199" s="1">
         <v>86928760</v>
@@ -6031,7 +6134,7 @@
       </c>
       <c r="B202" s="5">
         <f ca="1">RANDBETWEEN(81,82)</f>
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C202" s="1">
         <v>86928760</v>
@@ -6070,7 +6173,7 @@
       </c>
       <c r="B205" s="5">
         <f ca="1">RANDBETWEEN(111,112)</f>
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C205" s="1">
         <v>86928760</v>
@@ -6109,7 +6212,7 @@
       </c>
       <c r="B208" s="5">
         <f ca="1">RANDBETWEEN(21,22)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C208" s="1">
         <v>11293419</v>
@@ -6135,7 +6238,7 @@
       </c>
       <c r="B210" s="5">
         <f ca="1">RANDBETWEEN(41,44)</f>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C210" s="1">
         <v>11293419</v>
@@ -6148,7 +6251,7 @@
       </c>
       <c r="B211" s="5">
         <f ca="1">RANDBETWEEN(50,59)</f>
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C211" s="1">
         <v>11293419</v>
@@ -6174,7 +6277,7 @@
       </c>
       <c r="B213" s="5">
         <f ca="1">RANDBETWEEN(71,72)</f>
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C213" s="1">
         <v>11293419</v>
@@ -6200,7 +6303,7 @@
       </c>
       <c r="B215" s="5">
         <f ca="1">RANDBETWEEN(91,92)</f>
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C215" s="1">
         <v>11293419</v>
@@ -6213,7 +6316,7 @@
       </c>
       <c r="B216" s="5">
         <f ca="1">RANDBETWEEN(101,102)</f>
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C216" s="1">
         <v>11293419</v>
@@ -6278,7 +6381,7 @@
       </c>
       <c r="B221" s="5">
         <f ca="1">RANDBETWEEN(31,34)</f>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C221" s="1">
         <v>24896934</v>
@@ -6291,7 +6394,7 @@
       </c>
       <c r="B222" s="5">
         <f ca="1">RANDBETWEEN(41,44)</f>
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C222" s="1">
         <v>24896934</v>
@@ -6304,7 +6407,7 @@
       </c>
       <c r="B223" s="5">
         <f ca="1">RANDBETWEEN(50,59)</f>
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C223" s="1">
         <v>24896934</v>
@@ -6317,7 +6420,7 @@
       </c>
       <c r="B224" s="5">
         <f ca="1">RANDBETWEEN(61,63)</f>
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C224" s="1">
         <v>24896934</v>
@@ -6330,7 +6433,7 @@
       </c>
       <c r="B225" s="5">
         <f ca="1">RANDBETWEEN(71,72)</f>
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C225" s="1">
         <v>24896934</v>
@@ -6356,7 +6459,7 @@
       </c>
       <c r="B227" s="5">
         <f ca="1">RANDBETWEEN(91,92)</f>
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C227" s="1">
         <v>24896934</v>
@@ -6369,7 +6472,7 @@
       </c>
       <c r="B228" s="5">
         <f ca="1">RANDBETWEEN(101,102)</f>
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C228" s="1">
         <v>24896934</v>
@@ -6382,7 +6485,7 @@
       </c>
       <c r="B229" s="5">
         <f ca="1">RANDBETWEEN(111,112)</f>
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C229" s="1">
         <v>24896934</v>
@@ -6395,10 +6498,10 @@
       </c>
       <c r="B230" s="5">
         <f ca="1">RANDBETWEEN(1,6)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C230" s="1">
-        <v>65887539</v>
+        <v>11111111</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
@@ -6411,7 +6514,7 @@
         <v>11</v>
       </c>
       <c r="C231" s="1">
-        <v>65887539</v>
+        <v>11111111</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
@@ -6424,7 +6527,7 @@
         <v>21</v>
       </c>
       <c r="C232" s="1">
-        <v>65887539</v>
+        <v>11111111</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
@@ -6433,11 +6536,10 @@
         <v>233</v>
       </c>
       <c r="B233" s="5">
-        <f ca="1">RANDBETWEEN(31,34)</f>
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C233" s="1">
-        <v>65887539</v>
+        <v>11111111</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
@@ -6447,10 +6549,10 @@
       </c>
       <c r="B234" s="5">
         <f ca="1">RANDBETWEEN(41,44)</f>
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C234" s="1">
-        <v>65887539</v>
+        <v>11111111</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
@@ -6459,11 +6561,10 @@
         <v>235</v>
       </c>
       <c r="B235" s="5">
-        <f ca="1">RANDBETWEEN(50,59)</f>
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C235" s="1">
-        <v>65887539</v>
+        <v>11111111</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
@@ -6473,10 +6574,10 @@
       </c>
       <c r="B236" s="5">
         <f ca="1">RANDBETWEEN(61,63)</f>
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C236" s="1">
-        <v>65887539</v>
+        <v>11111111</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
@@ -6489,7 +6590,7 @@
         <v>71</v>
       </c>
       <c r="C237" s="1">
-        <v>65887539</v>
+        <v>11111111</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
@@ -6502,7 +6603,7 @@
         <v>82</v>
       </c>
       <c r="C238" s="1">
-        <v>65887539</v>
+        <v>11111111</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
@@ -6515,7 +6616,7 @@
         <v>92</v>
       </c>
       <c r="C239" s="1">
-        <v>65887539</v>
+        <v>11111111</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
@@ -6528,7 +6629,7 @@
         <v>101</v>
       </c>
       <c r="C240" s="1">
-        <v>65887539</v>
+        <v>11111111</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
@@ -6538,10 +6639,485 @@
       </c>
       <c r="B241" s="5">
         <f ca="1">RANDBETWEEN(111,112)</f>
+        <v>112</v>
+      </c>
+      <c r="C241" s="1">
+        <v>11111111</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A242" s="3">
+        <f t="shared" si="0"/>
+        <v>242</v>
+      </c>
+      <c r="B242" s="5">
+        <f ca="1">RANDBETWEEN(1,6)</f>
+        <v>6</v>
+      </c>
+      <c r="C242" s="1">
+        <v>22222222</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A243" s="3">
+        <f t="shared" ref="A243:A278" si="1">ROW()</f>
+        <v>243</v>
+      </c>
+      <c r="B243" s="5">
+        <f ca="1">RANDBETWEEN(11,12)</f>
+        <v>12</v>
+      </c>
+      <c r="C243" s="1">
+        <v>22222222</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A244" s="3">
+        <f t="shared" si="1"/>
+        <v>244</v>
+      </c>
+      <c r="B244" s="5">
+        <f ca="1">RANDBETWEEN(21,22)</f>
+        <v>21</v>
+      </c>
+      <c r="C244" s="1">
+        <v>22222222</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A245" s="3">
+        <f t="shared" si="1"/>
+        <v>245</v>
+      </c>
+      <c r="B245" s="5">
+        <v>32</v>
+      </c>
+      <c r="C245" s="1">
+        <v>22222222</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A246" s="3">
+        <f t="shared" si="1"/>
+        <v>246</v>
+      </c>
+      <c r="B246" s="5">
+        <f ca="1">RANDBETWEEN(41,44)</f>
+        <v>44</v>
+      </c>
+      <c r="C246" s="1">
+        <v>22222222</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A247" s="3">
+        <f t="shared" si="1"/>
+        <v>247</v>
+      </c>
+      <c r="B247" s="5">
+        <v>56</v>
+      </c>
+      <c r="C247" s="1">
+        <v>22222222</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A248" s="3">
+        <f t="shared" si="1"/>
+        <v>248</v>
+      </c>
+      <c r="B248" s="5">
+        <f ca="1">RANDBETWEEN(61,63)</f>
+        <v>61</v>
+      </c>
+      <c r="C248" s="1">
+        <v>22222222</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A249" s="3">
+        <f t="shared" si="1"/>
+        <v>249</v>
+      </c>
+      <c r="B249" s="5">
+        <f ca="1">RANDBETWEEN(71,72)</f>
+        <v>71</v>
+      </c>
+      <c r="C249" s="1">
+        <v>22222222</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A250" s="3">
+        <f t="shared" si="1"/>
+        <v>250</v>
+      </c>
+      <c r="B250" s="5">
+        <f ca="1">RANDBETWEEN(81,82)</f>
+        <v>82</v>
+      </c>
+      <c r="C250" s="1">
+        <v>22222222</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A251" s="3">
+        <f t="shared" si="1"/>
+        <v>251</v>
+      </c>
+      <c r="B251" s="5">
+        <f ca="1">RANDBETWEEN(91,92)</f>
+        <v>91</v>
+      </c>
+      <c r="C251" s="1">
+        <v>22222222</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A252" s="3">
+        <f t="shared" si="1"/>
+        <v>252</v>
+      </c>
+      <c r="B252" s="5">
+        <f ca="1">RANDBETWEEN(101,102)</f>
+        <v>101</v>
+      </c>
+      <c r="C252" s="1">
+        <v>22222222</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A253" s="3">
+        <f t="shared" si="1"/>
+        <v>253</v>
+      </c>
+      <c r="B253" s="5">
+        <f ca="1">RANDBETWEEN(111,112)</f>
+        <v>112</v>
+      </c>
+      <c r="C253" s="1">
+        <v>22222222</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A254" s="3">
+        <f t="shared" si="1"/>
+        <v>254</v>
+      </c>
+      <c r="B254" s="5">
+        <f ca="1">RANDBETWEEN(1,6)</f>
+        <v>3</v>
+      </c>
+      <c r="C254" s="1">
+        <v>33333333</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A255" s="3">
+        <f t="shared" si="1"/>
+        <v>255</v>
+      </c>
+      <c r="B255" s="5">
+        <f ca="1">RANDBETWEEN(11,12)</f>
+        <v>11</v>
+      </c>
+      <c r="C255" s="1">
+        <v>33333333</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A256" s="3">
+        <f t="shared" si="1"/>
+        <v>256</v>
+      </c>
+      <c r="B256" s="5">
+        <f ca="1">RANDBETWEEN(21,22)</f>
+        <v>22</v>
+      </c>
+      <c r="C256" s="1">
+        <v>33333333</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A257" s="3">
+        <f t="shared" si="1"/>
+        <v>257</v>
+      </c>
+      <c r="B257" s="5">
+        <v>32</v>
+      </c>
+      <c r="C257" s="1">
+        <v>33333333</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A258" s="3">
+        <f t="shared" si="1"/>
+        <v>258</v>
+      </c>
+      <c r="B258" s="5">
+        <f ca="1">RANDBETWEEN(41,44)</f>
+        <v>44</v>
+      </c>
+      <c r="C258" s="1">
+        <v>33333333</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A259" s="3">
+        <f t="shared" si="1"/>
+        <v>259</v>
+      </c>
+      <c r="B259" s="5">
+        <v>57</v>
+      </c>
+      <c r="C259" s="1">
+        <v>33333333</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A260" s="3">
+        <f t="shared" si="1"/>
+        <v>260</v>
+      </c>
+      <c r="B260" s="5">
+        <f ca="1">RANDBETWEEN(61,63)</f>
+        <v>61</v>
+      </c>
+      <c r="C260" s="1">
+        <v>33333333</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A261" s="3">
+        <f t="shared" si="1"/>
+        <v>261</v>
+      </c>
+      <c r="B261" s="5">
+        <f ca="1">RANDBETWEEN(71,72)</f>
+        <v>71</v>
+      </c>
+      <c r="C261" s="1">
+        <v>33333333</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A262" s="3">
+        <f t="shared" si="1"/>
+        <v>262</v>
+      </c>
+      <c r="B262" s="5">
+        <f ca="1">RANDBETWEEN(81,82)</f>
+        <v>82</v>
+      </c>
+      <c r="C262" s="1">
+        <v>33333333</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A263" s="3">
+        <f t="shared" si="1"/>
+        <v>263</v>
+      </c>
+      <c r="B263" s="5">
+        <f ca="1">RANDBETWEEN(91,92)</f>
+        <v>92</v>
+      </c>
+      <c r="C263" s="1">
+        <v>33333333</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A264" s="3">
+        <f t="shared" si="1"/>
+        <v>264</v>
+      </c>
+      <c r="B264" s="5">
+        <f ca="1">RANDBETWEEN(101,102)</f>
+        <v>102</v>
+      </c>
+      <c r="C264" s="1">
+        <v>33333333</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A265" s="3">
+        <f t="shared" si="1"/>
+        <v>265</v>
+      </c>
+      <c r="B265" s="5">
+        <f ca="1">RANDBETWEEN(111,112)</f>
         <v>111</v>
       </c>
-      <c r="C241" s="1">
-        <v>65887539</v>
+      <c r="C265" s="1">
+        <v>33333333</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A266" s="3">
+        <f t="shared" si="1"/>
+        <v>266</v>
+      </c>
+      <c r="B266" s="5">
+        <f ca="1">RANDBETWEEN(111,112)</f>
+        <v>111</v>
+      </c>
+      <c r="C266" s="1">
+        <v>33333333</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A267" s="3">
+        <f t="shared" si="1"/>
+        <v>267</v>
+      </c>
+      <c r="B267" s="5">
+        <f ca="1">RANDBETWEEN(1,6)</f>
+        <v>3</v>
+      </c>
+      <c r="C267" s="1">
+        <v>44444444</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A268" s="3">
+        <f t="shared" si="1"/>
+        <v>268</v>
+      </c>
+      <c r="B268" s="5">
+        <f ca="1">RANDBETWEEN(11,12)</f>
+        <v>11</v>
+      </c>
+      <c r="C268" s="1">
+        <v>44444444</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A269" s="3">
+        <f t="shared" si="1"/>
+        <v>269</v>
+      </c>
+      <c r="B269" s="5">
+        <f ca="1">RANDBETWEEN(21,22)</f>
+        <v>21</v>
+      </c>
+      <c r="C269" s="1">
+        <v>44444444</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A270" s="3">
+        <f t="shared" si="1"/>
+        <v>270</v>
+      </c>
+      <c r="B270" s="5">
+        <v>32</v>
+      </c>
+      <c r="C270" s="1">
+        <v>44444444</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A271" s="3">
+        <f t="shared" si="1"/>
+        <v>271</v>
+      </c>
+      <c r="B271" s="5">
+        <f ca="1">RANDBETWEEN(41,44)</f>
+        <v>43</v>
+      </c>
+      <c r="C271" s="1">
+        <v>44444444</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A272" s="3">
+        <f t="shared" si="1"/>
+        <v>272</v>
+      </c>
+      <c r="B272" s="5">
+        <v>58</v>
+      </c>
+      <c r="C272" s="1">
+        <v>44444444</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A273" s="3">
+        <f t="shared" si="1"/>
+        <v>273</v>
+      </c>
+      <c r="B273" s="5">
+        <f ca="1">RANDBETWEEN(61,63)</f>
+        <v>61</v>
+      </c>
+      <c r="C273" s="1">
+        <v>44444444</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A274" s="3">
+        <f t="shared" si="1"/>
+        <v>274</v>
+      </c>
+      <c r="B274" s="5">
+        <f ca="1">RANDBETWEEN(71,72)</f>
+        <v>71</v>
+      </c>
+      <c r="C274" s="1">
+        <v>44444444</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A275" s="3">
+        <f t="shared" si="1"/>
+        <v>275</v>
+      </c>
+      <c r="B275" s="5">
+        <f ca="1">RANDBETWEEN(81,82)</f>
+        <v>81</v>
+      </c>
+      <c r="C275" s="1">
+        <v>44444444</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A276" s="3">
+        <f t="shared" si="1"/>
+        <v>276</v>
+      </c>
+      <c r="B276" s="5">
+        <f ca="1">RANDBETWEEN(91,92)</f>
+        <v>91</v>
+      </c>
+      <c r="C276" s="1">
+        <v>44444444</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A277" s="3">
+        <f t="shared" si="1"/>
+        <v>277</v>
+      </c>
+      <c r="B277" s="5">
+        <f ca="1">RANDBETWEEN(101,102)</f>
+        <v>101</v>
+      </c>
+      <c r="C277" s="1">
+        <v>44444444</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A278" s="3">
+        <f t="shared" si="1"/>
+        <v>278</v>
+      </c>
+      <c r="B278" s="5">
+        <f ca="1">RANDBETWEEN(111,112)</f>
+        <v>112</v>
+      </c>
+      <c r="C278" s="1">
+        <v>44444444</v>
       </c>
     </row>
   </sheetData>

</xml_diff>